<commit_message>
fixed bug of mid classes
</commit_message>
<xml_diff>
--- a/individual_routines/L5CG2_routine_3rdSem.xlsx
+++ b/individual_routines/L5CG2_routine_3rdSem.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -607,17 +607,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>7:00-9:00</t>
+          <t>9:00-11:00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>5CS024</t>
+          <t>5CS022</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Collaborative Development</t>
+          <t>Human Computer Interaction</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -630,12 +630,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Mr. Raj Shrestha</t>
+          <t>Mr. Pravash Karki</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>LT-03 Walsall</t>
+          <t>LT-02 Telford</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -645,7 +645,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>L5CG(12+13+14)</t>
+          <t>L5CG(1+2+3+4)</t>
         </is>
       </c>
       <c r="K4" t="n">
@@ -665,17 +665,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>9:00-11:00</t>
+          <t>12:00-14:00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>5CS022</t>
+          <t>5CS020</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Human Computer Interaction</t>
+          <t>Distributed and Cloud Systems Programming</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -688,12 +688,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Mr. Pravash Karki</t>
+          <t>Mr. Sumanta Silwal</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>LT-02 Telford</t>
+          <t>LT-01 Wulfruna</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -718,22 +718,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>TUE</t>
+          <t>WED</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>12:00-14:00</t>
+          <t>9:30-11:30</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>5CS020</t>
+          <t>5CS024</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Distributed and Cloud Systems Programming</t>
+          <t>Collaborative Development</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -746,7 +746,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Mr. Sumanta Silwal</t>
+          <t>Mr. Udaya Kandel</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -781,17 +781,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>7:00-9:00</t>
+          <t>12:30-14:30</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>5CS022</t>
+          <t>5CS020</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Human Computer Interaction</t>
+          <t>Distributed and Cloud Systems Programming</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -799,17 +799,17 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Lecture</t>
+          <t>Tutorial</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Mr. Ayush Shakya</t>
+          <t>Mr. Prabin Sapkota</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>LT-01 Wulfruna</t>
+          <t>TR-03 Westbromwich</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -819,7 +819,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>L5CG(12+13+14)</t>
+          <t>L5CG2</t>
         </is>
       </c>
       <c r="K7" t="n">
@@ -834,22 +834,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>WED</t>
+          <t>THU</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>9:30-11:30</t>
+          <t>9:00-11:00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>5CS024</t>
+          <t>5CS022</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Collaborative Development</t>
+          <t>Human Computer Interaction</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -857,17 +857,17 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Lecture</t>
+          <t>Tutorial</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Mr. Udaya Kandel</t>
+          <t>Mr. Dipesh Shrestha</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>LT-01 Wulfruna</t>
+          <t>TR-02 Stafford</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -877,7 +877,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>L5CG(1+2+3+4)</t>
+          <t>L5CG2</t>
         </is>
       </c>
       <c r="K8" t="n">
@@ -892,22 +892,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>WED</t>
+          <t>FRI</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>12:30-14:30</t>
+          <t>10:00-12:00</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>5CS020</t>
+          <t>5CS024</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Distributed and Cloud Systems Programming</t>
+          <t>Collaborative Development</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -920,17 +920,17 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Mr. Prabin Sapkota</t>
+          <t>Mr. Anmol Adhikari</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>TR-03 Westbromwich</t>
+          <t>TR-09  Chandragiri</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>WLV</t>
+          <t>HCK</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -950,12 +950,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>THU</t>
+          <t>FRI</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>9:00-11:00</t>
+          <t>13:30-16:00</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -969,11 +969,11 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Tutorial</t>
+          <t>Workshop</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -983,7 +983,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>TR-02 Stafford</t>
+          <t>SR-03 Wolves</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1000,180 +1000,6 @@
         <v>5</v>
       </c>
       <c r="L10" t="inlineStr">
-        <is>
-          <t>BCS</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>THU</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>9:30-11:30</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>5CS020</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Distributed and Cloud Systems Programming</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>2</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Lecture</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Mr. Sumanta Silwal</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>LT-01 Wulfruna</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>WLV</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>L5CG(12+13+14)</t>
-        </is>
-      </c>
-      <c r="K11" t="n">
-        <v>5</v>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>BCS</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>FRI</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>10:00-12:00</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>5CS024</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Collaborative Development</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>2</v>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Tutorial</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Mr. Anmol Adhikari</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>TR-09  Chandragiri</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>HCK</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>L5CG2</t>
-        </is>
-      </c>
-      <c r="K12" t="n">
-        <v>5</v>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>BCS</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>FRI</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>13:30-16:00</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>5CS022</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Human Computer Interaction</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Workshop</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>Mr. Dipesh Shrestha</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>SR-03 Wolves</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>WLV</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>L5CG2</t>
-        </is>
-      </c>
-      <c r="K13" t="n">
-        <v>5</v>
-      </c>
-      <c r="L13" t="inlineStr">
         <is>
           <t>BCS</t>
         </is>

</xml_diff>